<commit_message>
fix csv formatting AGAIN
</commit_message>
<xml_diff>
--- a/power_data/20240212213025944.xlsx
+++ b/power_data/20240212213025944.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bdaha\Documents\GitHub\commapogo\power_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0781B086-0475-440C-8F9B-984B0342121A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F99CFC90-9017-4F7F-BA56-559BC7C4F391}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4632,7 +4632,7 @@
   <dimension ref="A1:H1116"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>